<commit_message>
[dataset] upload dataset statistics, bugs are categorized by operators and code elements
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/CATEGORIZED_BUGS/mutation_operators.xlsx
+++ b/experiment_results/SBFL_ONLY/CATEGORIZED_BUGS/mutation_operators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuanngokien/Desktop/Software_Analysis/configurable_system/InputPreparation/experiment_results/SBFL_ONLY/CATEGORIZED_BUGS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A530EE22-3CAD-BD4D-B77D-9276511AC90E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DFC76B-60B8-AE41-BE10-4A5F37C365A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{243BDA3A-3E7F-B543-BD56-8A47C6077E7C}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>ZipMe</t>
   </si>
   <si>
-    <t>{'ROR': 60, 'AORS': 28, 'COI': 2, 'AODU': 3, 'AOIU': 169, 'AODS': 29, 'AOIS': 2, 'COD': 1}</t>
-  </si>
-  <si>
     <t>GPL</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>ExamDB</t>
   </si>
   <si>
-    <t>{'AOIU': 346, 'ASRS': 61, 'AORS': 254, 'AODU': 94, 'AOIS': 207, 'COD': 172, 'ODL': 68, 'ROR': 41, 'COI': 36}</t>
-  </si>
-  <si>
     <t>BankAccountTP</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>ASSIGNMENT</t>
+  </si>
+  <si>
+    <t>{'AOIU': 155, 'AORS': 137, 'AOIS': 79, 'COD': 62, 'AODU': 43, 'ODL': 37, 'ASRS': 29, 'ROR': 15, 'COI': 8}</t>
+  </si>
+  <si>
+    <t>{'AOIU': 327, 'ROR': 146, 'COI': 68, 'AODU': 48, 'COD': 31, 'AORS': 28, 'AODS': 18, 'AOIS': 16}</t>
   </si>
 </sst>
 </file>
@@ -263,7 +263,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:shade val="70000"/>
+                  <a:shade val="90000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -285,7 +285,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:shade val="90000"/>
+                  <a:tint val="90000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -307,7 +307,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:tint val="90000"/>
+                  <a:tint val="70000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -329,7 +329,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:tint val="70000"/>
+                  <a:tint val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -345,98 +345,13 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:tint val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-1765-8244-A987-B2FB8DDA5AA6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.10150835850792687"/>
-                  <c:y val="0.11227797744794096"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-1765-8244-A987-B2FB8DDA5AA6}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.1103095050037044E-2"/>
-                  <c:y val="1.8885017421602788E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-1765-8244-A987-B2FB8DDA5AA6}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.10367937203299432"/>
-                  <c:y val="-8.1964251419792036E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-B216-984A-AC66-A1D260356148}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.17731184196597968"/>
-                  <c:y val="-0.16302340256248457"/>
+                  <c:x val="0.14947728649303452"/>
+                  <c:y val="-7.4315264007060414E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -452,66 +367,6 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.2640848797726552E-2"/>
-                  <c:y val="0.11092018985431698"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="rect">
-                      <a:avLst/>
-                    </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-1765-8244-A987-B2FB8DDA5AA6}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -520,23 +375,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr sz="1050"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -563,17 +408,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                </c15:spPr>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -609,22 +444,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>548</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>352</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2288</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>174</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,7 +479,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="22"/>
+        <c:firstSliceAng val="27"/>
       </c:pieChart>
       <c:spPr>
         <a:noFill/>
@@ -698,531 +533,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
-  <a:schemeClr val="accent3"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1233,10 +543,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1564,7 +874,7 @@
   <dimension ref="A4:H32"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C32" sqref="A27:C32"/>
+      <selection activeCell="C32" sqref="C27:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1590,10 +900,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1604,10 +914,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1618,10 +928,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1632,10 +942,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1646,10 +956,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1660,71 +970,71 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>534</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1216</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>352</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>372</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>173</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
@@ -1732,7 +1042,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>119</v>
@@ -1740,84 +1050,90 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>174</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>352</v>
+        <v>412</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1">
-        <v>548</v>
+        <f>SUM(B18,B19,B20)</f>
+        <v>506</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1">
+        <f>B21</f>
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1">
-        <v>130</v>
+        <f>B17</f>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1">
-        <v>352</v>
+        <f>B23</f>
+        <v>412</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1">
-        <v>2288</v>
+        <f>SUM(B12,B13,B14,B15,B16)</f>
+        <v>2007</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1">
-        <v>174</v>
+        <f>B22</f>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1838,7 +1154,7 @@
   <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1849,15 +1165,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
-        <v>548</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>119</v>
@@ -1865,34 +1181,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
-        <v>352</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
-        <v>2288</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
-        <v>174</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>